<commit_message>
Completed data collection of titres for LB and Kan
Medians are:
- DG011 #5
- DG012 #8
- SLM1042 #6 and SLM1042 #8
- SLM1043 #1 and SLM1043 #7
</commit_message>
<xml_diff>
--- a/Viable Titre/DG011-12_SLM142-43_17-09.xlsx
+++ b/Viable Titre/DG011-12_SLM142-43_17-09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1756,44 +1756,1340 @@
           <t>LB</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C37" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1e-06</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="F37" t="n">
+        <v>3</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3</v>
+      </c>
+      <c r="H37" t="n">
+        <v>26</v>
+      </c>
+      <c r="I37" t="n">
+        <v>27</v>
+      </c>
+      <c r="J37" t="n">
+        <v>268181818.1818181</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>DG011 #1</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F38" t="n">
+        <v>37</v>
+      </c>
+      <c r="G38" t="n">
+        <v>40</v>
+      </c>
+      <c r="H38" t="n">
+        <v>5</v>
+      </c>
+      <c r="I38" t="n">
+        <v>2</v>
+      </c>
+      <c r="J38" t="n">
+        <v>3818.181818181818</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>DG011 #2</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F39" t="n">
+        <v>7</v>
+      </c>
+      <c r="G39" t="n">
+        <v>2</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>409.0909090909091</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>DG011 #3</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F40" t="n">
+        <v>10</v>
+      </c>
+      <c r="G40" t="n">
+        <v>11</v>
+      </c>
+      <c r="H40" t="n">
+        <v>3</v>
+      </c>
+      <c r="I40" t="n">
+        <v>1</v>
+      </c>
+      <c r="J40" t="n">
+        <v>1136.363636363636</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>DG011 #4</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F41" t="n">
+        <v>12</v>
+      </c>
+      <c r="G41" t="n">
+        <v>8</v>
+      </c>
+      <c r="H41" t="n">
+        <v>2</v>
+      </c>
+      <c r="I41" t="n">
+        <v>2</v>
+      </c>
+      <c r="J41" t="n">
+        <v>1090.909090909091</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>DG011 #5</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F42" t="n">
+        <v>8</v>
+      </c>
+      <c r="G42" t="n">
+        <v>8</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1</v>
+      </c>
+      <c r="I42" t="n">
+        <v>3</v>
+      </c>
+      <c r="J42" t="n">
+        <v>909.090909090909</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>DG011 #6</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F43" t="n">
+        <v>2</v>
+      </c>
+      <c r="G43" t="n">
+        <v>2</v>
+      </c>
+      <c r="H43" t="n">
+        <v>1</v>
+      </c>
+      <c r="I43" t="n">
+        <v>2</v>
+      </c>
+      <c r="J43" t="n">
+        <v>318.1818181818181</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>DG011 #7</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F44" t="n">
+        <v>13</v>
+      </c>
+      <c r="G44" t="n">
+        <v>14</v>
+      </c>
+      <c r="H44" t="n">
+        <v>2</v>
+      </c>
+      <c r="I44" t="n">
+        <v>2</v>
+      </c>
+      <c r="J44" t="n">
+        <v>1409.090909090909</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>DG011 #8</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F45" t="n">
+        <v>3</v>
+      </c>
+      <c r="G45" t="n">
+        <v>7</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>DG011 #9</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F46" t="n">
+        <v>4</v>
+      </c>
+      <c r="G46" t="n">
+        <v>8</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="n">
+        <v>590.9090909090909</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>DG012 #1</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F47" t="n">
+        <v>29</v>
+      </c>
+      <c r="G47" t="n">
+        <v>32</v>
+      </c>
+      <c r="H47" t="n">
+        <v>8</v>
+      </c>
+      <c r="I47" t="n">
+        <v>3</v>
+      </c>
+      <c r="J47" t="n">
+        <v>3272.727272727273</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>DG012 #2</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F48" t="n">
+        <v>34</v>
+      </c>
+      <c r="G48" t="n">
+        <v>22</v>
+      </c>
+      <c r="H48" t="n">
+        <v>2</v>
+      </c>
+      <c r="I48" t="n">
+        <v>5</v>
+      </c>
+      <c r="J48" t="n">
+        <v>2863.636363636364</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>DG012 #3</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F49" t="n">
+        <v>23</v>
+      </c>
+      <c r="G49" t="n">
+        <v>18</v>
+      </c>
+      <c r="H49" t="n">
+        <v>1</v>
+      </c>
+      <c r="I49" t="n">
+        <v>2</v>
+      </c>
+      <c r="J49" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>DG012 #4</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F50" t="n">
+        <v>26</v>
+      </c>
+      <c r="G50" t="n">
+        <v>24</v>
+      </c>
+      <c r="H50" t="n">
+        <v>9</v>
+      </c>
+      <c r="I50" t="n">
+        <v>9</v>
+      </c>
+      <c r="J50" t="n">
+        <v>3090.909090909091</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>DG012 #5</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F51" t="n">
+        <v>21</v>
+      </c>
+      <c r="G51" t="n">
+        <v>25</v>
+      </c>
+      <c r="H51" t="n">
+        <v>5</v>
+      </c>
+      <c r="I51" t="n">
+        <v>9</v>
+      </c>
+      <c r="J51" t="n">
+        <v>2727.272727272727</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>DG012 #6</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F52" t="n">
+        <v>20</v>
+      </c>
+      <c r="G52" t="n">
+        <v>24</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="n">
+        <v>2</v>
+      </c>
+      <c r="J52" t="n">
+        <v>2090.909090909091</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>DG012 #7</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F53" t="n">
+        <v>17</v>
+      </c>
+      <c r="G53" t="n">
+        <v>13</v>
+      </c>
+      <c r="H53" t="n">
+        <v>2</v>
+      </c>
+      <c r="I53" t="n">
+        <v>3</v>
+      </c>
+      <c r="J53" t="n">
+        <v>1590.909090909091</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>DG012 #8</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D54" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F54" t="n">
+        <v>26</v>
+      </c>
+      <c r="G54" t="n">
+        <v>18</v>
+      </c>
+      <c r="H54" t="n">
+        <v>5</v>
+      </c>
+      <c r="I54" t="n">
+        <v>5</v>
+      </c>
+      <c r="J54" t="n">
+        <v>2454.545454545455</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>DG012 #9</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F55" t="n">
+        <v>24</v>
+      </c>
+      <c r="G55" t="n">
+        <v>23</v>
+      </c>
+      <c r="H55" t="n">
+        <v>3</v>
+      </c>
+      <c r="I55" t="n">
+        <v>3</v>
+      </c>
+      <c r="J55" t="n">
+        <v>2409.090909090909</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>SLM1042 #1</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F56" t="n">
+        <v>7</v>
+      </c>
+      <c r="G56" t="n">
+        <v>2</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>409.0909090909091</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>SLM1042 #2</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F57" t="n">
+        <v>8</v>
+      </c>
+      <c r="G57" t="n">
+        <v>11</v>
+      </c>
+      <c r="H57" t="n">
+        <v>1</v>
+      </c>
+      <c r="I57" t="n">
+        <v>2</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>SLM1042 #3</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F58" t="n">
+        <v>6</v>
+      </c>
+      <c r="G58" t="n">
+        <v>6</v>
+      </c>
+      <c r="H58" t="n">
+        <v>1</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>590.9090909090909</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>SLM1042 #4</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F59" t="n">
+        <v>7</v>
+      </c>
+      <c r="G59" t="n">
+        <v>4</v>
+      </c>
+      <c r="H59" t="n">
+        <v>1</v>
+      </c>
+      <c r="I59" t="n">
+        <v>1</v>
+      </c>
+      <c r="J59" t="n">
+        <v>590.9090909090909</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>SLM1042 #5</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F60" t="n">
+        <v>20</v>
+      </c>
+      <c r="G60" t="n">
+        <v>17</v>
+      </c>
+      <c r="H60" t="n">
+        <v>4</v>
+      </c>
+      <c r="I60" t="n">
+        <v>7</v>
+      </c>
+      <c r="J60" t="n">
+        <v>2181.818181818181</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>SLM1042 #6</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F61" t="n">
+        <v>8</v>
+      </c>
+      <c r="G61" t="n">
+        <v>5</v>
+      </c>
+      <c r="H61" t="n">
+        <v>1</v>
+      </c>
+      <c r="I61" t="n">
+        <v>3</v>
+      </c>
+      <c r="J61" t="n">
+        <v>772.7272727272726</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>SLM1042 #7</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F62" t="n">
+        <v>9</v>
+      </c>
+      <c r="G62" t="n">
+        <v>11</v>
+      </c>
+      <c r="H62" t="n">
+        <v>5</v>
+      </c>
+      <c r="I62" t="n">
+        <v>2</v>
+      </c>
+      <c r="J62" t="n">
+        <v>1227.272727272727</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>SLM1042 #8</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F63" t="n">
+        <v>9</v>
+      </c>
+      <c r="G63" t="n">
+        <v>6</v>
+      </c>
+      <c r="H63" t="n">
+        <v>1</v>
+      </c>
+      <c r="I63" t="n">
+        <v>1</v>
+      </c>
+      <c r="J63" t="n">
+        <v>772.7272727272726</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>SLM1042 #9</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F64" t="n">
+        <v>28</v>
+      </c>
+      <c r="G64" t="n">
+        <v>27</v>
+      </c>
+      <c r="H64" t="n">
+        <v>5</v>
+      </c>
+      <c r="I64" t="n">
+        <v>6</v>
+      </c>
+      <c r="J64" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>SLM1043 #1</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F65" t="n">
+        <v>23</v>
+      </c>
+      <c r="G65" t="n">
+        <v>17</v>
+      </c>
+      <c r="H65" t="n">
+        <v>1</v>
+      </c>
+      <c r="I65" t="n">
+        <v>2</v>
+      </c>
+      <c r="J65" t="n">
+        <v>1954.545454545455</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>SLM1043 #2</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F66" t="n">
+        <v>26</v>
+      </c>
+      <c r="G66" t="n">
+        <v>28</v>
+      </c>
+      <c r="H66" t="n">
+        <v>4</v>
+      </c>
+      <c r="I66" t="n">
+        <v>5</v>
+      </c>
+      <c r="J66" t="n">
+        <v>2863.636363636364</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>SLM1043 #3</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F67" t="n">
+        <v>15</v>
+      </c>
+      <c r="G67" t="n">
+        <v>18</v>
+      </c>
+      <c r="H67" t="n">
+        <v>3</v>
+      </c>
+      <c r="I67" t="n">
+        <v>3</v>
+      </c>
+      <c r="J67" t="n">
+        <v>1772.727272727272</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>SLM1043 #4</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F68" t="n">
+        <v>17</v>
+      </c>
+      <c r="G68" t="n">
+        <v>25</v>
+      </c>
+      <c r="H68" t="n">
+        <v>3</v>
+      </c>
+      <c r="I68" t="n">
+        <v>4</v>
+      </c>
+      <c r="J68" t="n">
+        <v>2227.272727272727</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>SLM1043 #5</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F69" t="n">
+        <v>21</v>
+      </c>
+      <c r="G69" t="n">
+        <v>24</v>
+      </c>
+      <c r="H69" t="n">
+        <v>1</v>
+      </c>
+      <c r="I69" t="n">
+        <v>3</v>
+      </c>
+      <c r="J69" t="n">
+        <v>2227.272727272727</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>SLM1043 #6</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D70" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F70" t="n">
+        <v>15</v>
+      </c>
+      <c r="G70" t="n">
+        <v>21</v>
+      </c>
+      <c r="H70" t="n">
+        <v>1</v>
+      </c>
+      <c r="I70" t="n">
+        <v>4</v>
+      </c>
+      <c r="J70" t="n">
+        <v>1863.636363636364</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>SLM1043 #7</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F71" t="n">
+        <v>17</v>
+      </c>
+      <c r="G71" t="n">
+        <v>21</v>
+      </c>
+      <c r="H71" t="n">
+        <v>2</v>
+      </c>
+      <c r="I71" t="n">
+        <v>3</v>
+      </c>
+      <c r="J71" t="n">
+        <v>1954.545454545455</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>SLM1043 #8</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D72" t="n">
+        <v>1</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F72" t="n">
+        <v>9</v>
+      </c>
+      <c r="G72" t="n">
+        <v>15</v>
+      </c>
+      <c r="H72" t="n">
+        <v>3</v>
+      </c>
+      <c r="I72" t="n">
+        <v>5</v>
+      </c>
+      <c r="J72" t="n">
+        <v>1454.545454545455</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>SLM1043 #9</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
         <is>
           <t>0.01</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>10e-7</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>10e-6</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>10e-1</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>10e-2</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>268181818.18181813</t>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>2409.090909090909</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
20-09 Median 4 strains mutation rates
data attached
fixed issue where volume was pre specified, no selected with drop down.

foxed issue where misspelling strains wouldn't retrieve the data, now added drop down.
</commit_message>
<xml_diff>
--- a/Viable Titre/DG011-12_SLM142-43_17-09.xlsx
+++ b/Viable Titre/DG011-12_SLM142-43_17-09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3052,44 +3052,332 @@
           <t>Kan</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
+      <c r="C73" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D73" t="n">
+        <v>1</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F73" t="n">
+        <v>22</v>
+      </c>
+      <c r="G73" t="n">
+        <v>24</v>
+      </c>
+      <c r="H73" t="n">
+        <v>3</v>
+      </c>
+      <c r="I73" t="n">
+        <v>4</v>
+      </c>
+      <c r="J73" t="n">
+        <v>2409.090909090909</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>DG011 #5</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>LB</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="E74" t="n">
+        <v>1e-06</v>
+      </c>
+      <c r="F74" t="n">
+        <v>177</v>
+      </c>
+      <c r="G74" t="n">
+        <v>177</v>
+      </c>
+      <c r="H74" t="n">
+        <v>18</v>
+      </c>
+      <c r="I74" t="n">
+        <v>18</v>
+      </c>
+      <c r="J74" t="n">
+        <v>177272727.2727272</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>DG012 #8</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>LB</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D75" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="E75" t="n">
+        <v>1e-06</v>
+      </c>
+      <c r="F75" t="n">
+        <v>255</v>
+      </c>
+      <c r="G75" t="n">
+        <v>255</v>
+      </c>
+      <c r="H75" t="n">
+        <v>32</v>
+      </c>
+      <c r="I75" t="n">
+        <v>32</v>
+      </c>
+      <c r="J75" t="n">
+        <v>260909090.9090908</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>SLM1042 #8</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>LB</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D76" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="E76" t="n">
+        <v>1e-06</v>
+      </c>
+      <c r="F76" t="n">
+        <v>232</v>
+      </c>
+      <c r="G76" t="n">
+        <v>232</v>
+      </c>
+      <c r="H76" t="n">
+        <v>22</v>
+      </c>
+      <c r="I76" t="n">
+        <v>22</v>
+      </c>
+      <c r="J76" t="n">
+        <v>230909090.9090908</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>SLM1043 #7</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>LB</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D77" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="E77" t="n">
+        <v>1e-06</v>
+      </c>
+      <c r="F77" t="n">
+        <v>139</v>
+      </c>
+      <c r="G77" t="n">
+        <v>139</v>
+      </c>
+      <c r="H77" t="n">
+        <v>7</v>
+      </c>
+      <c r="I77" t="n">
+        <v>7</v>
+      </c>
+      <c r="J77" t="n">
+        <v>132727272.7272727</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>DG011 #5</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D78" t="n">
+        <v>1</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F78" t="n">
+        <v>85</v>
+      </c>
+      <c r="G78" t="n">
+        <v>85</v>
+      </c>
+      <c r="H78" t="n">
+        <v>11</v>
+      </c>
+      <c r="I78" t="n">
+        <v>11</v>
+      </c>
+      <c r="J78" t="n">
+        <v>872.7272727272726</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>DG012 #8</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D79" t="n">
+        <v>1</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F79" t="n">
+        <v>175</v>
+      </c>
+      <c r="G79" t="n">
+        <v>175</v>
+      </c>
+      <c r="H79" t="n">
+        <v>22</v>
+      </c>
+      <c r="I79" t="n">
+        <v>22</v>
+      </c>
+      <c r="J79" t="n">
+        <v>1790.909090909091</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>SLM1042 #8</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D80" t="n">
+        <v>1</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F80" t="n">
+        <v>129</v>
+      </c>
+      <c r="G80" t="n">
+        <v>129</v>
+      </c>
+      <c r="H80" t="n">
+        <v>8</v>
+      </c>
+      <c r="I80" t="n">
+        <v>8</v>
+      </c>
+      <c r="J80" t="n">
+        <v>1245.454545454545</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>SLM1043 #7</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Kan</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
         <is>
           <t>10e-1</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="E81" t="inlineStr">
         <is>
           <t>10e-2</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>2409.090909090909</t>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>258</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>258</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>2527.272727272727</t>
         </is>
       </c>
     </row>

</xml_diff>